<commit_message>
Rename script for dist
</commit_message>
<xml_diff>
--- a/Output/cummulative_data.xlsx
+++ b/Output/cummulative_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1680" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -474,8 +474,8 @@
   </sheetPr>
   <dimension ref="A1:DG60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="DA70" sqref="DA70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>